<commit_message>
updated sponsors and team list
</commit_message>
<xml_diff>
--- a/public/assets/team_details.xlsx
+++ b/public/assets/team_details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\TeamWebsite\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2B8FF-5009-4A83-8110-4107332DD124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E97F82-2279-4977-AE32-CBCE571FE716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -118,21 +118,6 @@
     <t>https://github.com/Jugraunaqsingh</t>
   </si>
   <si>
-    <t>Akshat</t>
-  </si>
-  <si>
-    <t>Senior Core - Software</t>
-  </si>
-  <si>
-    <t>AIML RoboSoccer RL Programmer</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/akshatkhndelwal/</t>
-  </si>
-  <si>
-    <t>https://github.com/Akshatrix404</t>
-  </si>
-  <si>
     <t>Jaskanwar Bhatti</t>
   </si>
   <si>
@@ -175,93 +160,6 @@
     <t>https://github.com/GiT-Jay21</t>
   </si>
   <si>
-    <t>Lavnesh</t>
-  </si>
-  <si>
-    <t>Senior Core Electronics</t>
-  </si>
-  <si>
-    <t>Wiring brains into bots, because even robots need a genius</t>
-  </si>
-  <si>
-    <t>Siddharth</t>
-  </si>
-  <si>
-    <t>Senior core Software</t>
-  </si>
-  <si>
-    <t>ML enthusiast, Programmer</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/siddharth-sharan-08543229b?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
-  </si>
-  <si>
-    <t>https://github.com/sidSha22</t>
-  </si>
-  <si>
-    <t>Vishesh</t>
-  </si>
-  <si>
-    <t>Senior Core Hardware</t>
-  </si>
-  <si>
-    <t>My job? Making sure our machines don’t just work—they dominate!</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/vishesh-prasanna-sarapure?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
-  </si>
-  <si>
-    <t>https://github.com/VisheshPS</t>
-  </si>
-  <si>
-    <t>Kartikey</t>
-  </si>
-  <si>
-    <t>Senior core Hardware</t>
-  </si>
-  <si>
-    <t>I did boxing,football,taekwondo and now all my brain power goes into making a robot that'd play better football than me</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/kartikey-singh-484b46353?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
-  </si>
-  <si>
-    <t>Senior Core Management</t>
-  </si>
-  <si>
-    <t>ahh partially living (life support)</t>
-  </si>
-  <si>
-    <t>Vedant</t>
-  </si>
-  <si>
-    <t>Robotics, automation and design</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/vedant-chechani-5198a5236/</t>
-  </si>
-  <si>
-    <t>Janya Sirohi</t>
-  </si>
-  <si>
-    <t>helping robots get better at soccer—because if they’re going to take over, they might as well play a decent game.</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/janya-sirohi/</t>
-  </si>
-  <si>
-    <t>https://github.com/janyaexe</t>
-  </si>
-  <si>
-    <t>Hritam</t>
-  </si>
-  <si>
-    <t>Avg Robotics enjoyer, Snack Ethusiast</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/hritam-shrivastava-07679a28a?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
-  </si>
-  <si>
     <t>Chief Team Advisor</t>
   </si>
   <si>
@@ -317,12 +215,6 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/kunal-kundnani-452288274/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/lavnesh-rao-676327314/</t>
-  </si>
-  <si>
-    <t>Agatsya Mishra</t>
   </si>
   <si>
     <t>Ayushman Kar</t>
@@ -637,7 +529,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -674,7 +566,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -694,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
@@ -711,13 +603,13 @@
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>19</v>
@@ -753,13 +645,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
@@ -768,30 +660,30 @@
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>22</v>
@@ -806,30 +698,30 @@
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>25</v>
@@ -844,10 +736,10 @@
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>28</v>
@@ -864,152 +756,92 @@
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
       <c r="F19" s="3"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1032,37 +864,19 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>79</v>
-      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
       <c r="F21" s="3"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1108,16 +922,8 @@
     <hyperlink ref="E11" r:id="rId20" xr:uid="{3A8ADACC-9EFE-478F-BDDC-950D4CE87F88}"/>
     <hyperlink ref="B12" r:id="rId21" xr:uid="{7E3B7237-9AAD-403D-BF05-714F7AC2B926}"/>
     <hyperlink ref="E12" r:id="rId22" xr:uid="{326DEC11-AD78-43C4-AC2E-0DD182555EA3}"/>
-    <hyperlink ref="E13" r:id="rId23" xr:uid="{68803900-2C0A-4016-93DB-6B9820EB7F87}"/>
-    <hyperlink ref="E14" r:id="rId24" display="http://www.linkedin.com/in/lavnesh-rao-676327314" xr:uid="{FED285D6-9895-480B-8C4B-500B6F9E05DA}"/>
-    <hyperlink ref="E15" r:id="rId25" xr:uid="{9EA0609D-3DB1-458A-AF7C-842A2DE1FE2A}"/>
-    <hyperlink ref="E16" r:id="rId26" xr:uid="{67F35B34-DA3A-43A7-88B2-08E10A789A2B}"/>
-    <hyperlink ref="E17" r:id="rId27" xr:uid="{5F1A6031-5FD8-431B-9DB9-D75A9F359C7B}"/>
-    <hyperlink ref="E19" r:id="rId28" xr:uid="{C8B23FB7-9DA4-44FF-B4D9-911F96E19378}"/>
-    <hyperlink ref="E20" r:id="rId29" xr:uid="{C5966B04-DAC7-48AF-AD16-A0CCD90A6234}"/>
-    <hyperlink ref="E21" r:id="rId30" xr:uid="{136D837D-5FCA-4DB8-A980-9D50FA6A3D51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>